<commit_message>
clean up for june_2024
</commit_message>
<xml_diff>
--- a/June_2024/june_2024.xlsx
+++ b/June_2024/june_2024.xlsx
@@ -509,7 +509,9 @@
       <c r="B2" t="n">
         <v>264000</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>876874</v>
+      </c>
       <c r="D2" t="n">
         <v>1100000</v>
       </c>
@@ -1459,7 +1461,9 @@
       <c r="B20" t="n">
         <v>1310000</v>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>3149718</v>
+      </c>
       <c r="D20" t="n">
         <v>3100000</v>
       </c>
@@ -1775,7 +1779,9 @@
       <c r="B26" t="n">
         <v>413000</v>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>4559224</v>
+      </c>
       <c r="D26" t="n">
         <v>3500000</v>
       </c>
@@ -1985,7 +1991,9 @@
       <c r="B30" t="n">
         <v>22700</v>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>214083</v>
+      </c>
       <c r="D30" t="n">
         <v>288000</v>
       </c>
@@ -2036,7 +2044,9 @@
       <c r="B31" t="n">
         <v>4230000</v>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>42102199</v>
+      </c>
       <c r="D31" t="n">
         <v>60000000</v>
       </c>
@@ -2405,7 +2415,9 @@
       <c r="B38" t="n">
         <v>27000</v>
       </c>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>153682</v>
+      </c>
       <c r="D38" t="n">
         <v>157000</v>
       </c>
@@ -2509,7 +2521,9 @@
       <c r="B40" t="n">
         <v>58600</v>
       </c>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>270113</v>
+      </c>
       <c r="D40" t="n">
         <v>473000</v>
       </c>
@@ -2666,7 +2680,9 @@
       <c r="B43" t="n">
         <v>36600</v>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>201428</v>
+      </c>
       <c r="D43" t="n">
         <v>566000</v>
       </c>
@@ -2823,7 +2839,9 @@
       <c r="B46" t="n">
         <v>87900</v>
       </c>
-      <c r="C46" t="inlineStr"/>
+      <c r="C46" t="n">
+        <v>628842</v>
+      </c>
       <c r="D46" t="n">
         <v>1000000</v>
       </c>
@@ -2980,7 +2998,9 @@
       <c r="B49" t="n">
         <v>569000</v>
       </c>
-      <c r="C49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>7979486</v>
+      </c>
       <c r="D49" t="n">
         <v>9000000</v>
       </c>
@@ -3084,7 +3104,9 @@
       <c r="B51" t="n">
         <v>25200</v>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="n">
+        <v>153318</v>
+      </c>
       <c r="D51" t="n">
         <v>209000</v>
       </c>
@@ -3188,7 +3210,9 @@
       <c r="B53" t="n">
         <v>28300</v>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>99586</v>
+      </c>
       <c r="D53" t="n">
         <v>86000</v>
       </c>
@@ -3345,7 +3369,9 @@
       <c r="B56" t="n">
         <v>12200</v>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="n">
+        <v>36188</v>
+      </c>
       <c r="D56" t="n">
         <v>66000</v>
       </c>
@@ -3443,7 +3469,9 @@
       <c r="B58" t="n">
         <v>298000</v>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>1408781</v>
+      </c>
       <c r="D58" t="n">
         <v>3400000</v>
       </c>
@@ -3541,7 +3569,9 @@
       <c r="B60" t="n">
         <v>85400</v>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>663886</v>
+      </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
         <v>458400</v>
@@ -3643,7 +3673,9 @@
       <c r="B62" t="n">
         <v>190000</v>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>1181486</v>
+      </c>
       <c r="D62" t="n">
         <v>1700000</v>
       </c>
@@ -3747,7 +3779,9 @@
       <c r="B64" t="n">
         <v>34300</v>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>181441</v>
+      </c>
       <c r="D64" t="n">
         <v>1600000</v>
       </c>
@@ -3851,7 +3885,9 @@
       <c r="B66" t="n">
         <v>833000</v>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>17067899</v>
+      </c>
       <c r="D66" t="n">
         <v>18000000</v>
       </c>
@@ -3955,7 +3991,9 @@
       <c r="B68" t="n">
         <v>401000</v>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>451209</v>
+      </c>
       <c r="D68" t="n">
         <v>4300000</v>
       </c>
@@ -4112,7 +4150,9 @@
       <c r="B71" t="n">
         <v>28400</v>
       </c>
-      <c r="C71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>814720</v>
+      </c>
       <c r="D71" t="n">
         <v>2000000</v>
       </c>
@@ -4163,7 +4203,9 @@
       <c r="B72" t="n">
         <v>25200</v>
       </c>
-      <c r="C72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>375494</v>
+      </c>
       <c r="D72" t="n">
         <v>1700000</v>
       </c>
@@ -4214,7 +4256,9 @@
       <c r="B73" t="n">
         <v>27900</v>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" t="n">
+        <v>284268</v>
+      </c>
       <c r="D73" t="n">
         <v>2000000</v>
       </c>
@@ -4318,7 +4362,9 @@
       <c r="B75" t="n">
         <v>170000</v>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>328272</v>
+      </c>
       <c r="D75" t="n">
         <v>1600000</v>
       </c>
@@ -4528,7 +4574,9 @@
       <c r="B79" t="n">
         <v>178000</v>
       </c>
-      <c r="C79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>931206</v>
+      </c>
       <c r="D79" t="n">
         <v>1900000</v>
       </c>
@@ -4685,7 +4733,9 @@
       <c r="B82" t="n">
         <v>68700</v>
       </c>
-      <c r="C82" t="inlineStr"/>
+      <c r="C82" t="n">
+        <v>1641801</v>
+      </c>
       <c r="D82" t="n">
         <v>2400000</v>
       </c>
@@ -4789,7 +4839,9 @@
       <c r="B84" t="n">
         <v>13400</v>
       </c>
-      <c r="C84" t="inlineStr"/>
+      <c r="C84" t="n">
+        <v>120523</v>
+      </c>
       <c r="D84" t="n">
         <v>155000</v>
       </c>
@@ -4893,7 +4945,9 @@
       <c r="B86" t="n">
         <v>3290</v>
       </c>
-      <c r="C86" t="inlineStr"/>
+      <c r="C86" t="n">
+        <v>232091</v>
+      </c>
       <c r="D86" t="n">
         <v>287000</v>
       </c>
@@ -4997,7 +5051,9 @@
       <c r="B88" t="n">
         <v>14500</v>
       </c>
-      <c r="C88" t="inlineStr"/>
+      <c r="C88" t="n">
+        <v>119732</v>
+      </c>
       <c r="D88" t="n">
         <v>122000</v>
       </c>
@@ -5101,7 +5157,9 @@
       <c r="B90" t="n">
         <v>23900</v>
       </c>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" t="n">
+        <v>386157</v>
+      </c>
       <c r="D90" t="n">
         <v>471000</v>
       </c>
@@ -5205,7 +5263,9 @@
       <c r="B92" t="n">
         <v>691000</v>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="n">
+        <v>3392220</v>
+      </c>
       <c r="D92" t="n">
         <v>7000000</v>
       </c>
@@ -5309,7 +5369,9 @@
       <c r="B94" t="n">
         <v>8220000</v>
       </c>
-      <c r="C94" t="inlineStr"/>
+      <c r="C94" t="n">
+        <v>64446712</v>
+      </c>
       <c r="D94" t="n">
         <v>52000000</v>
       </c>
@@ -5572,7 +5634,9 @@
       <c r="B99" t="n">
         <v>41700</v>
       </c>
-      <c r="C99" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>467539</v>
+      </c>
       <c r="D99" t="n">
         <v>685000</v>
       </c>
@@ -5676,7 +5740,9 @@
       <c r="B101" t="n">
         <v>29900</v>
       </c>
-      <c r="C101" t="inlineStr"/>
+      <c r="C101" t="n">
+        <v>643908</v>
+      </c>
       <c r="D101" t="n">
         <v>810000</v>
       </c>
@@ -5833,7 +5899,9 @@
       <c r="B104" t="n">
         <v>109000</v>
       </c>
-      <c r="C104" t="inlineStr"/>
+      <c r="C104" t="n">
+        <v>2275929</v>
+      </c>
       <c r="D104" t="n">
         <v>4800000</v>
       </c>
@@ -5937,7 +6005,9 @@
       <c r="B106" t="n">
         <v>45100</v>
       </c>
-      <c r="C106" t="inlineStr"/>
+      <c r="C106" t="n">
+        <v>660209</v>
+      </c>
       <c r="D106" t="n">
         <v>1500000</v>
       </c>
@@ -6094,7 +6164,9 @@
       <c r="B109" t="n">
         <v>13300</v>
       </c>
-      <c r="C109" t="inlineStr"/>
+      <c r="C109" t="n">
+        <v>551428</v>
+      </c>
       <c r="D109" t="n">
         <v>873000</v>
       </c>
@@ -6251,7 +6323,9 @@
       <c r="B112" t="n">
         <v>80100</v>
       </c>
-      <c r="C112" t="inlineStr"/>
+      <c r="C112" t="n">
+        <v>1643384</v>
+      </c>
       <c r="D112" t="n">
         <v>1700000</v>
       </c>
@@ -6461,7 +6535,9 @@
       <c r="B116" t="n">
         <v>40800</v>
       </c>
-      <c r="C116" t="inlineStr"/>
+      <c r="C116" t="n">
+        <v>655645</v>
+      </c>
       <c r="D116" t="n">
         <v>1000000</v>
       </c>
@@ -6565,7 +6641,9 @@
       <c r="B118" t="n">
         <v>124000</v>
       </c>
-      <c r="C118" t="inlineStr"/>
+      <c r="C118" t="n">
+        <v>1555897</v>
+      </c>
       <c r="D118" t="n">
         <v>1500000</v>
       </c>
@@ -6669,7 +6747,9 @@
       <c r="B120" t="n">
         <v>21500</v>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" t="n">
+        <v>513387</v>
+      </c>
       <c r="D120" t="n">
         <v>763000</v>
       </c>
@@ -6773,7 +6853,9 @@
       <c r="B122" t="n">
         <v>32300</v>
       </c>
-      <c r="C122" t="inlineStr"/>
+      <c r="C122" t="n">
+        <v>817865</v>
+      </c>
       <c r="D122" t="n">
         <v>1100000</v>
       </c>
@@ -6877,7 +6959,9 @@
       <c r="B124" t="n">
         <v>119000</v>
       </c>
-      <c r="C124" t="inlineStr"/>
+      <c r="C124" t="n">
+        <v>1592530</v>
+      </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="n">
         <v>535300</v>
@@ -7085,7 +7169,9 @@
       <c r="B128" t="n">
         <v>40900</v>
       </c>
-      <c r="C128" t="inlineStr"/>
+      <c r="C128" t="n">
+        <v>1017847</v>
+      </c>
       <c r="D128" t="n">
         <v>2300000</v>
       </c>
@@ -7136,7 +7222,9 @@
       <c r="B129" t="n">
         <v>66200</v>
       </c>
-      <c r="C129" t="inlineStr"/>
+      <c r="C129" t="n">
+        <v>1702043</v>
+      </c>
       <c r="D129" t="n">
         <v>1800000</v>
       </c>
@@ -7605,7 +7693,9 @@
       <c r="B138" t="n">
         <v>13400</v>
       </c>
-      <c r="C138" t="inlineStr"/>
+      <c r="C138" t="n">
+        <v>176102</v>
+      </c>
       <c r="D138" t="n">
         <v>151000</v>
       </c>
@@ -7709,7 +7799,9 @@
       <c r="B140" t="n">
         <v>19600</v>
       </c>
-      <c r="C140" t="inlineStr"/>
+      <c r="C140" t="n">
+        <v>226540</v>
+      </c>
       <c r="D140" t="n">
         <v>337000</v>
       </c>
@@ -7919,7 +8011,9 @@
       <c r="B144" t="n">
         <v>19200</v>
       </c>
-      <c r="C144" t="inlineStr"/>
+      <c r="C144" t="n">
+        <v>137937</v>
+      </c>
       <c r="D144" t="n">
         <v>276000</v>
       </c>
@@ -7970,7 +8064,9 @@
       <c r="B145" t="n">
         <v>28100</v>
       </c>
-      <c r="C145" t="inlineStr"/>
+      <c r="C145" t="n">
+        <v>263073</v>
+      </c>
       <c r="D145" t="n">
         <v>407000</v>
       </c>
@@ -8021,7 +8117,9 @@
       <c r="B146" t="n">
         <v>9070</v>
       </c>
-      <c r="C146" t="inlineStr"/>
+      <c r="C146" t="n">
+        <v>165265</v>
+      </c>
       <c r="D146" t="n">
         <v>112000</v>
       </c>
@@ -8602,7 +8700,9 @@
       <c r="B157" t="n">
         <v>13700</v>
       </c>
-      <c r="C157" t="inlineStr"/>
+      <c r="C157" t="n">
+        <v>163657</v>
+      </c>
       <c r="D157" t="n">
         <v>233000</v>
       </c>
@@ -9024,7 +9124,9 @@
       <c r="B165" t="n">
         <v>155000</v>
       </c>
-      <c r="C165" t="inlineStr"/>
+      <c r="C165" t="n">
+        <v>4516809</v>
+      </c>
       <c r="D165" t="n">
         <v>4900000</v>
       </c>
@@ -10241,7 +10343,9 @@
       <c r="B188" t="n">
         <v>165000</v>
       </c>
-      <c r="C188" t="inlineStr"/>
+      <c r="C188" t="n">
+        <v>1405486</v>
+      </c>
       <c r="D188" t="n">
         <v>3300000</v>
       </c>
@@ -11193,7 +11297,9 @@
       <c r="B206" t="n">
         <v>279000</v>
       </c>
-      <c r="C206" t="inlineStr"/>
+      <c r="C206" t="n">
+        <v>2355097</v>
+      </c>
       <c r="D206" t="n">
         <v>3200000</v>
       </c>
@@ -12569,7 +12675,9 @@
       <c r="B232" t="n">
         <v>61000</v>
       </c>
-      <c r="C232" t="inlineStr"/>
+      <c r="C232" t="n">
+        <v>939746</v>
+      </c>
       <c r="D232" t="n">
         <v>1800000</v>
       </c>
@@ -13256,7 +13364,9 @@
       <c r="B245" t="n">
         <v>36000</v>
       </c>
-      <c r="C245" t="inlineStr"/>
+      <c r="C245" t="n">
+        <v>578898</v>
+      </c>
       <c r="D245" t="n">
         <v>852000</v>
       </c>
@@ -13625,7 +13735,9 @@
       <c r="B252" t="n">
         <v>58000</v>
       </c>
-      <c r="C252" t="inlineStr"/>
+      <c r="C252" t="n">
+        <v>969603</v>
+      </c>
       <c r="D252" t="n">
         <v>790000</v>
       </c>
@@ -14312,7 +14424,9 @@
       <c r="B265" t="n">
         <v>129000</v>
       </c>
-      <c r="C265" t="inlineStr"/>
+      <c r="C265" t="n">
+        <v>450149</v>
+      </c>
       <c r="D265" t="n">
         <v>419000</v>
       </c>
@@ -14787,7 +14901,9 @@
       <c r="B274" t="n">
         <v>1700000</v>
       </c>
-      <c r="C274" t="inlineStr"/>
+      <c r="C274" t="n">
+        <v>16316774</v>
+      </c>
       <c r="D274" t="n">
         <v>28000000</v>
       </c>
@@ -15633,7 +15749,9 @@
       <c r="B290" t="n">
         <v>30700</v>
       </c>
-      <c r="C290" t="inlineStr"/>
+      <c r="C290" t="n">
+        <v>299341</v>
+      </c>
       <c r="D290" t="n">
         <v>455000</v>
       </c>
@@ -15684,7 +15802,9 @@
       <c r="B291" t="n">
         <v>15400</v>
       </c>
-      <c r="C291" t="inlineStr"/>
+      <c r="C291" t="n">
+        <v>212126</v>
+      </c>
       <c r="D291" t="n">
         <v>144000</v>
       </c>
@@ -16000,7 +16120,9 @@
       <c r="B297" t="n">
         <v>1060</v>
       </c>
-      <c r="C297" t="inlineStr"/>
+      <c r="C297" t="n">
+        <v>133758</v>
+      </c>
       <c r="D297" t="n">
         <v>115000</v>
       </c>

</xml_diff>